<commit_message>
fix: set exit to reset button after starting survey, .gitignore, README updates
</commit_message>
<xml_diff>
--- a/Responses/John_Survey_P5555555_responses.xlsx
+++ b/Responses/John_Survey_P5555555_responses.xlsx
@@ -3315,7 +3315,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>&lt;missing&gt;</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -9642,7 +9642,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>&lt;missing&gt;</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>